<commit_message>
Supplementary Material and Figure patches
</commit_message>
<xml_diff>
--- a/manuscript/supplementary tables/suppl_tables.xlsx
+++ b/manuscript/supplementary tables/suppl_tables.xlsx
@@ -1714,12 +1714,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>COVID-19 severity</t>
+          <t>N COVID-19 patients</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>no: 100% (n = 9)</t>
+          <t>0% (n = 0)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>